<commit_message>
A10 sample, resize imgs and Entry insert
</commit_message>
<xml_diff>
--- a/A1 - escoria limpa/29-09-2023_12-30-07/tratamento1.xlsx
+++ b/A1 - escoria limpa/29-09-2023_12-30-07/tratamento1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F06415F-EA78-4257-B085-9FA0F7EC6C90}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9E5C69-8B57-4E55-964E-8CCDC819E8F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cru" sheetId="1" r:id="rId1"/>
@@ -15,10 +15,10 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Cru!$B$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Cru!$B$2:$B$105</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Processado!$B$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Processado!$B$2:$B$91</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Processado!$E$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Processado!$E$2:$E$91</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Processado!$E$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Processado!$E$2:$E$91</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Processado!$B$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Processado!$B$2:$B$91</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
   <si>
     <t>Id</t>
   </si>
@@ -279,12 +279,21 @@
   <si>
     <t>Estatística descritiva</t>
   </si>
+  <si>
+    <t>Cobrim. S brilho</t>
+  </si>
+  <si>
+    <t>Media S brilho</t>
+  </si>
+  <si>
+    <t>Desv. Pad. S brilho</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,6 +344,13 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -350,7 +366,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -415,12 +431,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -471,9 +500,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -485,6 +511,14 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2309,7 +2343,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Processado!$F$10:$F$11</c:f>
+              <c:f>Processado!$G$12:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2324,7 +2358,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Processado!$F$2,Processado!$F$2)</c:f>
+              <c:f>(Processado!$G$2,Processado!$G$2)</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2685,9 +2719,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -2696,15 +2729,29 @@
             <c:v>F. Observada.</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>normalidade!$I$4:$I$10</c:f>
@@ -2764,6 +2811,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3C7C-41E0-9BCB-63F08E8A130B}"/>
@@ -2777,15 +2825,29 @@
             <c:v>F. Normal.</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>normalidade!$M$4:$M$10</c:f>
@@ -2816,6 +2878,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-3C7C-41E0-9BCB-63F08E8A130B}"/>
@@ -2830,11 +2893,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="200"/>
-        <c:overlap val="-20"/>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="1539222943"/>
         <c:axId val="1539223359"/>
-      </c:barChart>
+      </c:lineChart>
       <c:catAx>
         <c:axId val="1539222943"/>
         <c:scaling>
@@ -2939,12 +3002,7 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -3190,7 +3248,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3228,7 +3286,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{AE582C71-A888-454F-86A2-796C8767D210}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>Pixels Agregados</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3256,7 +3314,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3294,7 +3352,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{BDF0065E-0469-4BFC-B593-BB490CDEB64D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>Cobrimento</cx:v>
             </cx:txData>
           </cx:tx>
@@ -7874,13 +7932,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>518820</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>93120</xdr:rowOff>
@@ -7952,13 +8010,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>594360</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>495960</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>93120</xdr:rowOff>
@@ -7990,13 +8048,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>518820</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>169320</xdr:rowOff>
@@ -8068,13 +8126,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>594360</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>495960</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>169320</xdr:rowOff>
@@ -8106,13 +8164,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>81600</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>87360</xdr:rowOff>
@@ -8569,8 +8627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U200"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10407,10 +10465,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70EAAED-2E1F-4803-8270-B1973955EBA5}">
-  <dimension ref="A1:G200"/>
+  <dimension ref="A1:H200"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10420,11 +10478,12 @@
     <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -10440,14 +10499,17 @@
       <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -10463,15 +10525,19 @@
       <c r="E2" s="3">
         <v>5.2631578947368398</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="29">
+        <f>IF(B2=0,"",100*(C2)/B2)</f>
+        <v>5.2631578947368425</v>
+      </c>
+      <c r="G2" s="10">
         <f>AVERAGE(E2:E91)</f>
         <v>2.6083048803511621</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -10487,15 +10553,19 @@
       <c r="E3" s="3">
         <v>4.2695106291910401</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="29">
+        <f t="shared" ref="F3:F66" si="0">IF(B3=0,"",100*(C3)/B3)</f>
+        <v>4.2695106291910401</v>
+      </c>
+      <c r="G3" s="10">
         <f>_xlfn.STDEV.S(E2:E91)</f>
         <v>2.424044822973245</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -10511,14 +10581,19 @@
       <c r="E4" s="3">
         <v>1.8209996125532699</v>
       </c>
-      <c r="F4" s="11">
-        <v>15</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F4" s="29">
+        <f t="shared" si="0"/>
+        <v>1.8209996125532739</v>
+      </c>
+      <c r="G4" s="30">
+        <f>AVERAGE(F2:F200)</f>
+        <v>2.6083048803511648</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -10534,14 +10609,19 @@
       <c r="E5" s="3">
         <v>2.93456894130862</v>
       </c>
-      <c r="F5" s="11">
-        <v>232</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F5" s="29">
+        <f t="shared" si="0"/>
+        <v>2.9345689413086213</v>
+      </c>
+      <c r="G5" s="30">
+        <f>_xlfn.STDEV.S(F2:F200)</f>
+        <v>2.424044822973245</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -10557,84 +10637,101 @@
       <c r="E6" s="3">
         <v>8.0284783761266301</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="29">
+        <f t="shared" si="0"/>
+        <v>8.0284783761266372</v>
+      </c>
+      <c r="G6" s="11">
+        <v>10</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>14659</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1324</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>9.0319939968619902</v>
+      </c>
+      <c r="F7" s="29">
+        <f t="shared" si="0"/>
+        <v>9.0319939968619956</v>
+      </c>
+      <c r="G7" s="11">
+        <v>221</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>17303</v>
+      </c>
+      <c r="C8" s="3">
+        <v>247</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1.4274981217129901</v>
+      </c>
+      <c r="F8" s="29">
+        <f t="shared" si="0"/>
+        <v>1.4274981217129978</v>
+      </c>
+      <c r="G8" s="12">
         <f>MIN(E2:E200)</f>
         <v>4.0562466197944798E-2</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3">
-        <v>14659</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1324</v>
-      </c>
-      <c r="D7" s="3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>17179</v>
+      </c>
+      <c r="C9" s="3">
+        <v>859</v>
+      </c>
+      <c r="D9" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="3">
-        <v>9.0319939968619902</v>
-      </c>
-      <c r="F7" s="12">
+      <c r="E9" s="3">
+        <v>5.0002910530298603</v>
+      </c>
+      <c r="F9" s="29">
+        <f t="shared" si="0"/>
+        <v>5.0002910530298621</v>
+      </c>
+      <c r="G9" s="12">
         <f>MAX(E2:E200)</f>
         <v>9.0319939968619902</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3">
-        <v>17303</v>
-      </c>
-      <c r="C8" s="3">
-        <v>247</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1.4274981217129901</v>
-      </c>
-      <c r="F8" s="13">
-        <f>100*F3/F2</f>
-        <v>92.935639588531927</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3">
-        <v>17179</v>
-      </c>
-      <c r="C9" s="3">
-        <v>859</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>5.0002910530298603</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="24"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -10650,14 +10747,19 @@
       <c r="E10" s="3">
         <v>4.3384697130712002</v>
       </c>
-      <c r="F10" s="11">
-        <v>0</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F10" s="29">
+        <f t="shared" si="0"/>
+        <v>4.3384697130712011</v>
+      </c>
+      <c r="G10" s="13">
+        <f>100*G3/G2</f>
+        <v>92.935639588531927</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -10673,50 +10775,71 @@
       <c r="E11" s="3">
         <v>5.1613368945354798</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="29">
+        <f t="shared" si="0"/>
+        <v>5.1613368945354798</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="23"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>12471</v>
+      </c>
+      <c r="C12" s="3">
+        <v>299</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2.3975623446395602</v>
+      </c>
+      <c r="F12" s="29">
+        <f t="shared" si="0"/>
+        <v>2.3975623446395637</v>
+      </c>
+      <c r="G12" s="11">
+        <v>0</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>21109</v>
+      </c>
+      <c r="C13" s="3">
+        <v>699</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3.3113837699559401</v>
+      </c>
+      <c r="F13" s="29">
+        <f t="shared" si="0"/>
+        <v>3.3113837699559427</v>
+      </c>
+      <c r="G13" s="11">
         <f>COUNT(A2:A200)</f>
         <v>25</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="H13" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3">
-        <v>12471</v>
-      </c>
-      <c r="C12" s="3">
-        <v>299</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>2.3975623446395602</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3">
-        <v>21109</v>
-      </c>
-      <c r="C13" s="3">
-        <v>699</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3">
-        <v>3.3113837699559401</v>
-      </c>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -10732,9 +10855,13 @@
       <c r="E14" s="3">
         <v>2.1256495040151102</v>
       </c>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F14" s="29">
+        <f t="shared" si="0"/>
+        <v>2.1256495040151155</v>
+      </c>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -10750,8 +10877,12 @@
       <c r="E15" s="3">
         <v>2.3450413223140401</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F15" s="29">
+        <f t="shared" si="0"/>
+        <v>2.3450413223140494</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -10767,8 +10898,12 @@
       <c r="E16" s="3">
         <v>0.22199556008879801</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="29">
+        <f t="shared" si="0"/>
+        <v>0.22199556008879823</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -10784,8 +10919,12 @@
       <c r="E17" s="3">
         <v>0.65478355765732998</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="29">
+        <f t="shared" si="0"/>
+        <v>0.65478355765732998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -10801,8 +10940,12 @@
       <c r="E18" s="3">
         <v>0.96982174784634501</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" s="29">
+        <f t="shared" si="0"/>
+        <v>0.96982174784634556</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -10818,8 +10961,12 @@
       <c r="E19" s="3">
         <v>0.12329611617234</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="29">
+        <f t="shared" si="0"/>
+        <v>0.12329611617234057</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -10835,8 +10982,12 @@
       <c r="E20" s="3">
         <v>1.6903969428007799</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" s="29">
+        <f t="shared" si="0"/>
+        <v>1.690396942800789</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -10852,8 +11003,12 @@
       <c r="E21" s="3">
         <v>0.67745197168857396</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" s="29">
+        <f t="shared" si="0"/>
+        <v>0.67745197168857429</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -10869,8 +11024,12 @@
       <c r="E22" s="3">
         <v>0.35365442910070699</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" s="29">
+        <f t="shared" si="0"/>
+        <v>0.35365442910070732</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -10886,8 +11045,12 @@
       <c r="E23" s="3">
         <v>0.82579835885642605</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" s="29">
+        <f t="shared" si="0"/>
+        <v>0.82579835885642605</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -10903,8 +11066,12 @@
       <c r="E24" s="3">
         <v>1.0088765494857801</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" s="29">
+        <f t="shared" si="0"/>
+        <v>1.0088765494857859</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -10920,8 +11087,12 @@
       <c r="E25" s="3">
         <v>1.1850421348314599</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25" s="29">
+        <f t="shared" si="0"/>
+        <v>1.1850421348314606</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -10937,1228 +11108,1928 @@
       <c r="E26" s="3">
         <v>4.0562466197944798E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26" s="29">
+        <f t="shared" si="0"/>
+        <v>4.0562466197944833E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F37" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F38" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F39" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F41" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F42" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F43" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F44" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F45" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F46" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F47" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F48" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F49" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F50" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F51" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F52" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F53" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F54" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F55" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F56" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F57" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F58" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F59" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F60" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F61" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F62" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F63" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F64" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F65" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F66" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F67" s="29" t="str">
+        <f t="shared" ref="F67:F130" si="1">IF(B67=0,"",100*(C67)/B67)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F68" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F69" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F70" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F71" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F72" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F73" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F74" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F75" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F76" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F77" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F78" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F79" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F80" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F81" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F82" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F83" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F84" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F85" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F86" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F87" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F88" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F89" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F90" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F91" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F92" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F93" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F94" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F95" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F96" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F97" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F98" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F99" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F100" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F101" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F102" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F103" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F104" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F105" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F106" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F107" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F108" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F109" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F110" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F111" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F112" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F113" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F114" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F115" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F116" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F117" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F118" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F119" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F120" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F121" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F122" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F123" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F124" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F125" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F126" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F127" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F128" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F129" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
       <c r="D130" s="3"/>
       <c r="E130" s="3"/>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F130" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
       <c r="D131" s="3"/>
       <c r="E131" s="3"/>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F131" s="29" t="str">
+        <f t="shared" ref="F131:F194" si="2">IF(B131=0,"",100*(C131)/B131)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
       <c r="D132" s="3"/>
       <c r="E132" s="3"/>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F132" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
       <c r="D133" s="3"/>
       <c r="E133" s="3"/>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F133" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" s="3"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
       <c r="D134" s="3"/>
       <c r="E134" s="3"/>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F134" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
       <c r="D135" s="3"/>
       <c r="E135" s="3"/>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F135" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="3"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
       <c r="D136" s="3"/>
       <c r="E136" s="3"/>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F136" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="3"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
       <c r="D137" s="3"/>
       <c r="E137" s="3"/>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F137" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
       <c r="D138" s="3"/>
       <c r="E138" s="3"/>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F138" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
       <c r="D139" s="3"/>
       <c r="E139" s="3"/>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F139" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="3"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
       <c r="D140" s="3"/>
       <c r="E140" s="3"/>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F140" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="3"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
       <c r="D141" s="3"/>
       <c r="E141" s="3"/>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F141" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="3"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
       <c r="D142" s="3"/>
       <c r="E142" s="3"/>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F142" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="3"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
       <c r="D143" s="3"/>
       <c r="E143" s="3"/>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F143" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="3"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
       <c r="E144" s="3"/>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F144" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="3"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
       <c r="D145" s="3"/>
       <c r="E145" s="3"/>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F145" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="3"/>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
       <c r="D146" s="3"/>
       <c r="E146" s="3"/>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F146" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="3"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
       <c r="D147" s="3"/>
       <c r="E147" s="3"/>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F147" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="3"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
       <c r="D148" s="3"/>
       <c r="E148" s="3"/>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F148" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="3"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
       <c r="D149" s="3"/>
       <c r="E149" s="3"/>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F149" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="3"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
       <c r="D150" s="3"/>
       <c r="E150" s="3"/>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F150" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" s="3"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
       <c r="D151" s="3"/>
       <c r="E151" s="3"/>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F151" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" s="3"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
       <c r="D152" s="3"/>
       <c r="E152" s="3"/>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F152" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" s="3"/>
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
       <c r="D153" s="3"/>
       <c r="E153" s="3"/>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F153" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" s="3"/>
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
       <c r="D154" s="3"/>
       <c r="E154" s="3"/>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F154" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" s="3"/>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
       <c r="D155" s="3"/>
       <c r="E155" s="3"/>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F155" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" s="3"/>
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
       <c r="D156" s="3"/>
       <c r="E156" s="3"/>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F156" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" s="3"/>
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
       <c r="D157" s="3"/>
       <c r="E157" s="3"/>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F157" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" s="3"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
       <c r="E158" s="3"/>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F158" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" s="3"/>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
       <c r="D159" s="3"/>
       <c r="E159" s="3"/>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F159" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" s="3"/>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
       <c r="D160" s="3"/>
       <c r="E160" s="3"/>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F160" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" s="3"/>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
       <c r="D161" s="3"/>
       <c r="E161" s="3"/>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F161" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162" s="3"/>
       <c r="B162" s="3"/>
       <c r="C162" s="3"/>
       <c r="D162" s="3"/>
       <c r="E162" s="3"/>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F162" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" s="3"/>
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
       <c r="D163" s="3"/>
       <c r="E163" s="3"/>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F163" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164" s="3"/>
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
       <c r="D164" s="3"/>
       <c r="E164" s="3"/>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F164" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165" s="3"/>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
       <c r="D165" s="3"/>
       <c r="E165" s="3"/>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F165" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166" s="3"/>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
       <c r="D166" s="3"/>
       <c r="E166" s="3"/>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F166" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167" s="3"/>
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
       <c r="D167" s="3"/>
       <c r="E167" s="3"/>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F167" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168" s="3"/>
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
       <c r="D168" s="3"/>
       <c r="E168" s="3"/>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F168" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169" s="3"/>
       <c r="B169" s="3"/>
       <c r="C169" s="3"/>
       <c r="D169" s="3"/>
       <c r="E169" s="3"/>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F169" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170" s="3"/>
       <c r="B170" s="3"/>
       <c r="C170" s="3"/>
       <c r="D170" s="3"/>
       <c r="E170" s="3"/>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F170" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171" s="3"/>
       <c r="B171" s="3"/>
       <c r="C171" s="3"/>
       <c r="D171" s="3"/>
       <c r="E171" s="3"/>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F171" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172" s="3"/>
       <c r="B172" s="3"/>
       <c r="C172" s="3"/>
       <c r="D172" s="3"/>
       <c r="E172" s="3"/>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F172" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173" s="3"/>
       <c r="B173" s="3"/>
       <c r="C173" s="3"/>
       <c r="D173" s="3"/>
       <c r="E173" s="3"/>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F173" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174" s="3"/>
       <c r="B174" s="3"/>
       <c r="C174" s="3"/>
       <c r="D174" s="3"/>
       <c r="E174" s="3"/>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F174" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175" s="3"/>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
       <c r="D175" s="3"/>
       <c r="E175" s="3"/>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F175" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176" s="3"/>
       <c r="B176" s="3"/>
       <c r="C176" s="3"/>
       <c r="D176" s="3"/>
       <c r="E176" s="3"/>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F176" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177" s="3"/>
       <c r="B177" s="3"/>
       <c r="C177" s="3"/>
       <c r="D177" s="3"/>
       <c r="E177" s="3"/>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F177" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178" s="3"/>
       <c r="B178" s="3"/>
       <c r="C178" s="3"/>
       <c r="D178" s="3"/>
       <c r="E178" s="3"/>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F178" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179" s="3"/>
       <c r="B179" s="3"/>
       <c r="C179" s="3"/>
       <c r="D179" s="3"/>
       <c r="E179" s="3"/>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F179" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180" s="3"/>
       <c r="B180" s="3"/>
       <c r="C180" s="3"/>
       <c r="D180" s="3"/>
       <c r="E180" s="3"/>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F180" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181" s="3"/>
       <c r="B181" s="3"/>
       <c r="C181" s="3"/>
       <c r="D181" s="3"/>
       <c r="E181" s="3"/>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F181" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182" s="3"/>
       <c r="B182" s="3"/>
       <c r="C182" s="3"/>
       <c r="D182" s="3"/>
       <c r="E182" s="3"/>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F182" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183" s="3"/>
       <c r="B183" s="3"/>
       <c r="C183" s="3"/>
       <c r="D183" s="3"/>
       <c r="E183" s="3"/>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F183" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184" s="3"/>
       <c r="B184" s="3"/>
       <c r="C184" s="3"/>
       <c r="D184" s="3"/>
       <c r="E184" s="3"/>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F184" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185" s="3"/>
       <c r="B185" s="3"/>
       <c r="C185" s="3"/>
       <c r="D185" s="3"/>
       <c r="E185" s="3"/>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F185" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186" s="3"/>
       <c r="B186" s="3"/>
       <c r="C186" s="3"/>
       <c r="D186" s="3"/>
       <c r="E186" s="3"/>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F186" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" s="3"/>
       <c r="B187" s="3"/>
       <c r="C187" s="3"/>
       <c r="D187" s="3"/>
       <c r="E187" s="3"/>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F187" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188" s="3"/>
       <c r="B188" s="3"/>
       <c r="C188" s="3"/>
       <c r="D188" s="3"/>
       <c r="E188" s="3"/>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F188" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189" s="3"/>
       <c r="B189" s="3"/>
       <c r="C189" s="3"/>
       <c r="D189" s="3"/>
       <c r="E189" s="3"/>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F189" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190" s="3"/>
       <c r="B190" s="3"/>
       <c r="C190" s="3"/>
       <c r="D190" s="3"/>
       <c r="E190" s="3"/>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F190" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191" s="3"/>
       <c r="B191" s="3"/>
       <c r="C191" s="3"/>
       <c r="D191" s="3"/>
       <c r="E191" s="3"/>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F191" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192" s="3"/>
       <c r="B192" s="3"/>
       <c r="C192" s="3"/>
       <c r="D192" s="3"/>
       <c r="E192" s="3"/>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F192" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A193" s="3"/>
       <c r="B193" s="3"/>
       <c r="C193" s="3"/>
       <c r="D193" s="3"/>
       <c r="E193" s="3"/>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F193" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194" s="3"/>
       <c r="B194" s="3"/>
       <c r="C194" s="3"/>
       <c r="D194" s="3"/>
       <c r="E194" s="3"/>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F194" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195" s="3"/>
       <c r="B195" s="3"/>
       <c r="C195" s="3"/>
       <c r="D195" s="3"/>
       <c r="E195" s="3"/>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F195" s="29" t="str">
+        <f t="shared" ref="F195:F200" si="3">IF(B195=0,"",100*(C195)/B195)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196" s="3"/>
       <c r="B196" s="3"/>
       <c r="C196" s="3"/>
       <c r="D196" s="3"/>
       <c r="E196" s="3"/>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F196" s="29" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197" s="3"/>
       <c r="B197" s="3"/>
       <c r="C197" s="3"/>
       <c r="D197" s="3"/>
       <c r="E197" s="3"/>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F197" s="29" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A198" s="3"/>
       <c r="B198" s="3"/>
       <c r="C198" s="3"/>
       <c r="D198" s="3"/>
       <c r="E198" s="3"/>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F198" s="29" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199" s="3"/>
       <c r="B199" s="3"/>
       <c r="C199" s="3"/>
       <c r="D199" s="3"/>
       <c r="E199" s="3"/>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F199" s="29" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200" s="3"/>
       <c r="B200" s="3"/>
       <c r="C200" s="3"/>
       <c r="D200" s="3"/>
       <c r="E200" s="3"/>
+      <c r="F200" s="29" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="G11:H11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12171,7 +13042,7 @@
   <dimension ref="B2:V12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12196,29 +13067,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="H2" s="25" t="s">
+      <c r="C2" s="25"/>
+      <c r="H2" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="P2" s="26" t="s">
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="P2" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="U2" s="26" t="s">
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="U2" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="V2" s="26"/>
+      <c r="V2" s="25"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B3" s="19" t="s">
@@ -12269,7 +13140,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="15">
-        <f>Processado!F2</f>
+        <f>Processado!G2</f>
         <v>2.6083048803511621</v>
       </c>
       <c r="D4" s="15"/>
@@ -12328,7 +13199,7 @@
         <v>18</v>
       </c>
       <c r="C5" s="15">
-        <f>Processado!F3</f>
+        <f>Processado!G3</f>
         <v>2.424044822973245</v>
       </c>
       <c r="D5" s="15"/>
@@ -12386,7 +13257,7 @@
         <v>33</v>
       </c>
       <c r="C6" s="15">
-        <f>Processado!F6</f>
+        <f>Processado!G8</f>
         <v>4.0562466197944798E-2</v>
       </c>
       <c r="D6" s="15"/>
@@ -12445,7 +13316,7 @@
         <v>34</v>
       </c>
       <c r="C7" s="15">
-        <f>Processado!F7</f>
+        <f>Processado!G9</f>
         <v>9.0319939968619902</v>
       </c>
       <c r="D7" s="15"/>
@@ -12660,11 +13531,11 @@
         <f t="shared" si="4"/>
         <v>0.10061835804479335</v>
       </c>
-      <c r="U10" s="27" t="str">
+      <c r="U10" s="26" t="str">
         <f>IF(S11&lt;V9,"Há indícios de normalidade","NÃO há indícios de normalidade")</f>
         <v>NÃO há indícios de normalidade</v>
       </c>
-      <c r="V10" s="27"/>
+      <c r="V10" s="26"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B11" s="17" t="s">
@@ -12692,12 +13563,12 @@
         <f>SUM(S4:S10)</f>
         <v>15.00002765900148</v>
       </c>
-      <c r="U11" s="28"/>
-      <c r="V11" s="28"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="27"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="U12" s="28"/>
-      <c r="V12" s="28"/>
+      <c r="U12" s="27"/>
+      <c r="V12" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>